<commit_message>
Interaction terms section 3.2.4
</commit_message>
<xml_diff>
--- a/NC_NR_VC_VR/DEG_Count.xlsx
+++ b/NC_NR_VC_VR/DEG_Count.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindz/BeeVirusDiet/NC_NR_VC_VR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindz/CompareViz/NC_NR_VC_VR/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1720" windowWidth="21460" windowHeight="9340" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="1720" windowWidth="24540" windowHeight="9340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,7 +451,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B7" sqref="B7"/>
+      <selection pane="topRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
edgeR on honeybee paper data
</commit_message>
<xml_diff>
--- a/NC_NR_VC_VR/DEG_Count.xlsx
+++ b/NC_NR_VC_VR/DEG_Count.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1720" windowWidth="24540" windowHeight="9340" tabRatio="500"/>
+    <workbookView xWindow="6440" yWindow="460" windowWidth="18840" windowHeight="10100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>DESeq2-m1</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>limmaVoom-Diet</t>
+  </si>
+  <si>
+    <t>Light green indicates significant mortality differences</t>
+  </si>
+  <si>
+    <t>Dark green indiciates significant IAPV differences</t>
   </si>
 </sst>
 </file>
@@ -125,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,7 +146,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,11 +173,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -447,11 +461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E6" sqref="E6"/>
+      <selection pane="topRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,43 +516,43 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>178</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>135</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>96</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>327</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -546,7 +560,7 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>376</v>
       </c>
       <c r="D4">
@@ -562,23 +576,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>774</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>677</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>535</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>143</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <f>47+108</f>
         <v>155</v>
       </c>
@@ -587,7 +601,7 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>941</v>
       </c>
       <c r="D6">
@@ -604,23 +618,23 @@
         <v>358</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3">
         <v>955</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>839</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>682</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>8</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <f>140+91</f>
         <v>231</v>
       </c>
@@ -657,6 +671,16 @@
       </c>
       <c r="M9">
         <v>1119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>